<commit_message>
Mindre opdatering efter første møde
</commit_message>
<xml_diff>
--- a/dandem_export_v1_0_0.xlsx
+++ b/dandem_export_v1_0_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,112 +488,86 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ReferralFreeChoice</t>
+          <t>NPU</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fritvalgshenvisning modtaget
-</t>
+          <t>Neuropsykologisk undersøgelse (NPU)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Patienter der er omvisiteret via fritvalgsordning til primær udredning jf. henvisningstype, da skal datoen for fritvalgshenvisningen oplyses. Fritvalgshenvisning kan gives ved lang ventetid.</t>
+          <t>Er NPU udført i udredningsenhedens regi, uddelegeret derfra eller blevet gennemlæst/vurderet af udredningsenhedens neuropsykologer og fundet velgennemført?
+**Testen skal være udført inden for de seneste 12 mdr.**</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>InformDiagnosis</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Denne dato er ekstrem vigtig og der skal gøres en stor indsats for at validere denne dato. Denne dato kobles bl.a. med henvsiningsdato og første kontakt dato i udredningsforløbet identificeret i LPR ved procedurekoden ZZ1500. Herudfra bestemmes ventetid og udredningstid, hvilke er ekstremt vigtige parametre for patient og pårørende og dermed ventidsgarantier regionerne bør leve op til. 
-Datoen er den dato, hvor alle undersøgelser, der er blevet lavet i udredningsforløbet foreligger og er vurderet/beskrevet og dermed kan føre til en konklusiv diagnose på det bedst mulige kliniske grundlag.
-</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>CT_Scan</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dato for diagnosesamtale defineres som den dag patienten første gang informeres om en diagnostisk konklusion. Dette er normalt ved en ambulant konsultation. Se eksempler nedenfor. Det skal ses fra patienten synsvinkel: ”Hvornår fik jeg første gang noget at vide om diagnose og evt. behandling.
-Hvis der gives svar per brev (f. eks hvis patienten ikke ønsker at møde op, eller der er aftalt brevsvar) anvendes dato for afgivelse af dette svar.
-Hvis patienten aflyser midt i et udredningsforløb, anvendes den dato hvor patienten afsluttes journalmæssigt.
-Hvis patienten dør under udredningsforløb, anvendes dødsdato.
-Hvis patienten efter den initiale udredning informeres om, at der er depression / depressive symptomer (og evt. sættes i behandling) vil dette være dato for diagnose. Dette også selv om man klinisk kan have en mistanke om en bagvedliggende demenssygdom, men hvor diagnose først kan stilles når depressionen er behandlet.</t>
+          <t>Forelægger der CT-scanning af cerebrum og evt. adgang til  billeder foretaget indenfor 24 måneder før diagnosesamtaledatoen.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ReferralCommunalCoordinator</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Kommunal demenskoordinator henvisning</t>
+          <t>MR_Scan</t>
         </is>
       </c>
     </row>
@@ -610,7 +584,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Der skal svares Ja, hvis patienten er blevet tilbudt henvisning. Både hvis patient/pårørende ønsker dette sat i værk eller hvis de ikke ønsker dette sat i værk.</t>
+          <t>Forelægger der MR-scanning af cerebrum og evt. adgang til  billeder foretaget indenfor 24 måneder før diagnosesamtaledatoen.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -622,141 +596,50 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Activity</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Referral</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Henvisningstype  / Pt. ønsker ikke udredning.
-Henvisningstypen er afgørende for, hvorledes patienten indgår i indikatorberegningen.</t>
+          <t>NPHAssessment</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>StatusCode</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
-        <is>
-          <t>Hvis 'Omvisiteret' er valgt, skal der angives en dato.</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "primaer_demensudredning_henvist_direkte" | "second_opinion" | "patient_oensker_ikke_yderligere_undersoegelser" | "omvisiteret_fritvalgspatient_til_primaer_udredning" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>NPHAssessment</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ActivityCode</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
         <is>
           <t>Er der udført normal-tryks-hydrocephalus (NPH)-udredning? Udredningen foretages, hvis man mistænker forhøjet intrakranielt tryk som årsag til kognigitiv deficit.
 Kan i de fleste implementeringer stå på 'nej' som standard.</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Activity</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>MR_Scan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>StatusCode</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Forelægger der MR-scanning af cerebrum og evt. adgang til  billeder foretaget indenfor 24 måneder før diagnosesamtaledatoen.</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>OfferedDementiaMedication</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Er patienten blevet tilbudt demensmedicin?
 Ved Ja forstås, at der i udredningsforløbet for demens er tilbudt behandling med én af følgende relevante medicintyper, som patienten skal påbegynde behandling med eller allerede er i behandling med følgende relevante medicintyper:
@@ -767,94 +650,211 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>StatusCode</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ReferralCommunalCoordinator</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kommunal demenskoordinator henvisning</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>StatusCode</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Der skal svares Ja, hvis patienten er blevet tilbudt henvisning. Både hvis patient/pårørende ønsker dette sat i værk eller hvis de ikke ønsker dette sat i værk.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Referral</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Henvisningstype  / Pt. ønsker ikke udredning.
+Henvisningstypen er afgørende for, hvorledes patienten indgår i indikatorberegningen.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "primaer_demensudredning_henvist_direkte" | "second_opinion" | "patient_oensker_ikke_yderligere_undersoegelser" | "omvisiteret_fritvalgspatient_til_primaer_udredning" | </t>
+        </is>
+      </c>
+    </row>
     <row r="16">
       <c r="D16" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Hvis 'Omvisiteret' er valgt, skal der angives en dato.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>NPU</t>
+          <t>ReferralFreeChoice</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Neuropsykologisk undersøgelse (NPU)</t>
+          <t xml:space="preserve">Fritvalgshenvisning modtaget
+</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Er NPU udført i udredningsenhedens regi, uddelegeret derfra eller blevet gennemlæst/vurderet af udredningsenhedens neuropsykologer og fundet velgennemført?
-**Testen skal være udført inden for de seneste 12 mdr.**</t>
+          <t>Patienter der er omvisiteret via fritvalgsordning til primær udredning jf. henvisningstype, da skal datoen for fritvalgshenvisningen oplyses. Fritvalgshenvisning kan gives ved lang ventetid.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Activity</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CT_Scan</t>
+          <t>InformDiagnosis</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Denne dato er ekstrem vigtig og der skal gøres en stor indsats for at validere denne dato. Denne dato kobles bl.a. med henvsiningsdato og første kontakt dato i udredningsforløbet identificeret i LPR ved procedurekoden ZZ1500. Herudfra bestemmes ventetid og udredningstid, hvilke er ekstremt vigtige parametre for patient og pårørende og dermed ventidsgarantier regionerne bør leve op til. 
+Datoen er den dato, hvor alle undersøgelser, der er blevet lavet i udredningsforløbet foreligger og er vurderet/beskrevet og dermed kan føre til en konklusiv diagnose på det bedst mulige kliniske grundlag.
+</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
         <is>
-          <t>StatusCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Forelægger der CT-scanning af cerebrum og evt. adgang til  billeder foretaget indenfor 24 måneder før diagnosesamtaledatoen.</t>
+          <t>Dato for diagnosesamtale defineres som den dag patienten første gang informeres om en diagnostisk konklusion. Dette er normalt ved en ambulant konsultation. Se eksempler nedenfor. Det skal ses fra patienten synsvinkel: ”Hvornår fik jeg første gang noget at vide om diagnose og evt. behandling.
+Hvis der gives svar per brev (f. eks hvis patienten ikke ønsker at møde op, eller der er aftalt brevsvar) anvendes dato for afgivelse af dette svar.
+Hvis patienten aflyser midt i et udredningsforløb, anvendes den dato hvor patienten afsluttes journalmæssigt.
+Hvis patienten dør under udredningsforløb, anvendes dødsdato.
+Hvis patienten efter den initiale udredning informeres om, at der er depression / depressive symptomer (og evt. sættes i behandling) vil dette være dato for diagnose. Dette også selv om man klinisk kan have en mistanke om en bagvedliggende demenssygdom, men hvor diagnose først kan stilles når depressionen er behandlet.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -866,374 +866,295 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>MMSE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Mini mental status examination (MMSE) er uden sammenligning det hyppigst anvendte kognitive screeningsinstrument i ind- og udland og indgår som rutineundersøgelse ved demensudredning.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MCE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Multicultural Cognitive Examination (MCE) er udviklet som et så vidt muligt kulturuafhængigt eller tværkulturelt screeningsinstrument for demens. MCE giver flere og mere nuancerede oplysninger om det kognitive funktionsniveau end fx RUDAS alene og udgør et velegnet supplement ved tværkulturel demensudredning.  
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Trinvold_DSQIID</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Trindvold/DSQIID er instrumenter der anvendes til vurdering af patienter med samtidig Downs syndrom eller anden mental retardering og mistanke om erhvervet demenssygdom.
+Dette instrument anvendes, når det ikke er muligt at anvende de sædvanlige instrumenter grundet mental retardering m.fl.
+**I tilfælde af denne er positiv, er der ikke behov for at udføre de andre tests. (LISTE AF TESTS)**</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>StatusCode</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MoCa</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Montreal Cognitive Assessment (MoCA) er udviklet med henblik på at identificere mild cognitive impairment (let kognitiv svækkelse; MCI).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CAMcog</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambridge Cognitive Examination (CAMCOG) er udviklet med henblik på at bidrage til at diagnosticere demens i et tidligt stadium og giver væsentligt flere oplysninger end fx MMSE. 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 105</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>DAD</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Disability Assessment for Dementia (DAD) er udviklet af en gruppe canadiske ergo- og fysioterapeuter med henblik på vurdering af praktisk funktionsevne hos hjemmeboende patienter med Alzheimers sygdom. Instrumentet er følsomt over for ændringer i funktionsevne.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 40</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>FAQ_IADL</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">Functional Activities Questionnaire (FAQ IADL) er udviklet med henblik på – via oplysninger fra pårørende – at opnå en hurtig og systematisk vurdering af patientens praktiske funktionsevne i hverdagen.
 </t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>DAD</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The Disability Assessment for Dementia (DAD) er udviklet af en gruppe canadiske ergo- og fysioterapeuter med henblik på vurdering af praktisk funktionsevne hos hjemmeboende patienter med Alzheimers sygdom. Instrumentet er følsomt over for ændringer i funktionsevne.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 40</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>BASIC</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Brief Assessment of Impaired Cognition (BASIC) er udviklet til rettidig identifikation af kognitiv svækkelse og demens.</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 25</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>CAMcog</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambridge Cognitive Examination (CAMCOG) er udviklet med henblik på at bidrage til at diagnosticere demens i et tidligt stadium og giver væsentligt flere oplysninger end fx MMSE. 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 105</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>MCE</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Multicultural Cognitive Examination (MCE) er udviklet som et så vidt muligt kulturuafhængigt eller tværkulturelt screeningsinstrument for demens. MCE giver flere og mere nuancerede oplysninger om det kognitive funktionsniveau end fx RUDAS alene og udgør et velegnet supplement ved tværkulturel demensudredning.  
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>RUDAS</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The Rowland Universal Dementia Assessment Scale (RUDAS) er udviklet som et så vidt muligt kulturuafhængigt eller tværkulturelt screeningsinstrument for demens. 
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>MoCa</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The Montreal Cognitive Assessment (MoCA) er udviklet med henblik på at identificere mild cognitive impairment (let kognitiv svækkelse; MCI).
-</t>
-        </is>
-      </c>
-    </row>
     <row r="34">
       <c r="D34" t="inlineStr">
         <is>
+          <t>StatusCode</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Var der en pårørende / professionel omsorgsperson involveret i vurderingen af FAQ_ADL?
+Da demente ikke altid selv har indsigt i eget funktionsniveau, da inddrages pårørende eller andre, som kender patienten indgående. Der markeres ”Ja” hvis der har været en pårørende og/eller professionel omsorgsperson (der kender patienten til at kunne svare på FAQ_ADL vurdering) ved forundersøgelse.</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="36">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>ACE</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Addenbrooke’s Cognitive Examination (ACE) giver flere og mere nuancerede oplysninger om det kognitive funktionsniveau end fx MMSE alene og udgør et velegnet supplement ved demensudredning.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="D36" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CognitiveImpairment</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Habituel kognitiv funktion: Test inden for alders- og uddannelseskorrigeret normalområde og præmorbid funktion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
         <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>ADSC_ADL</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Alzheimer's Disease Cooperative Study(ADCS)-ADL er udviklet med henblik på vurdering af praktisk funktionsevne hos patienter med Alzheimers sygdom.</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 78</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>MMSE</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Mini mental status examination (MMSE) er uden sammenligning det hyppigst anvendte kognitive screeningsinstrument i ind- og udland og indgår som rutineundersøgelse ved demensudredning.</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>CognitiveImpairment</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Habituel kognitiv funktion: Test inden for alders- og uddannelseskorrigeret normalområde og præmorbid funktion.</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>str, Enum</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>*Kognitiv svækkelse, ikke dement*
 Kognitiv svækkelse i et eller flere domæner, men ikke dement (normal ADL). Det er ikke  afgørende om patienten har svigt indenfor ét eller flere kognitive domæner, men om patienten trods svigt opretholder et normalt dagligt funktionsniveau. Den kognitive svækkelse kan være på såvel organisk som non-organisk baggrund.
@@ -1247,24 +1168,185 @@
 NIA-AA kriterier for demens skal være opfyldte og ADL påvirkning er svær jf. ICD-10 kriterier</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t xml:space="preserve">Enums/Udfald: | "kognitiv_intakt" | "kognitiv_svaekkelse" | "demens__let__grad" | "demens__moderat__grad" | "demens_svaer_grad" | </t>
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ACE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Addenbrooke’s Cognitive Examination (ACE) giver flere og mere nuancerede oplysninger om det kognitive funktionsniveau end fx MMSE alene og udgør et velegnet supplement ved demensudredning.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RUDAS</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Rowland Universal Dementia Assessment Scale (RUDAS) er udviklet som et så vidt muligt kulturuafhængigt eller tværkulturelt screeningsinstrument for demens. 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 30</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ADSC_ADL</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Alzheimer's Disease Cooperative Study(ADCS)-ADL er udviklet med henblik på vurdering af praktisk funktionsevne hos patienter med Alzheimers sygdom.</t>
+        </is>
+      </c>
+    </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>StatusCode</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Var der en pårørende / professionel omsorgsperson involveret i vurderingen af ADSC_ADL?
+Da demente ikke altid selv har indsigt i eget funktionsniveau, da inddrages pårørende eller andre, som kender patienten indgående. Der markeres ”Ja” hvis der har været en pårørende og/eller professionel omsorgsperson (der kender patienten til at kunne svare på ADSC_ADL vurdering) ved forundersøgelse.</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 78</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BASIC</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Brief Assessment of Impaired Cognition (BASIC) er udviklet til rettidig identifikation af kognitiv svækkelse og demens.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>Diagnosis</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B47" t="inlineStr">
         <is>
           <t>EtiologicalDiagnosis</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>Hvis Graden af kognitiv påvirkning ikke er svarende til Habituel kognitiv funktion, da skal Ætiologisk diagnose angives, hvis det er muligt. 
 Den sygdomsspecifikke diagnose, der registres skal være den anførte diagnose i journalen og som er kommunikeret til patient/pårørende. Ved flere konkurrerende ætiologier indberettes den ætiologi, der bedst beskriver den dominerende kliniske tilstand. 
@@ -1316,18 +1398,18 @@
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="D44" t="inlineStr">
+    <row r="48">
+      <c r="D48" t="inlineStr">
         <is>
           <t>DiagnosisCode</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>str, Enum</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t xml:space="preserve">Enums/Udfald: | "alzheimer_sygdom" | "lewy_body_sygdom" | "parkinson_sygdom" | "cerebrovaskulaer_sygdom" | "mixed_alzheimer_cerebrovaskulaer" | "frontotemporal_demens" | "atypisk_parkinson_msa_cbs_psp" | "normaltryks_hydrocephalus_nph" | "huntingtons_sygdom" | "alkohol" | "anden_specifik_neurodegenerativ_sygdom" | "anden__ikke_neurodegenerativ_sygdom" | "psykiatrisk_sygdom" | "uafklaret_aetiologi" | </t>
         </is>

</xml_diff>